<commit_message>
Adding ExcelReader utility and updated Excel data file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marb6\git\repository\ExcelDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35BFDE7-9982-42DA-8F39-36B3F0A4293F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>firstname</t>
   </si>
@@ -37,12 +38,6 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
     <t>A234wd</t>
   </si>
   <si>
@@ -64,18 +59,6 @@
     <t>Rupee</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -98,12 +81,36 @@
   </si>
   <si>
     <t>runmode</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Byrne</t>
+  </si>
+  <si>
+    <t>Alana</t>
+  </si>
+  <si>
+    <t>Curran</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Jones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,7 +421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -425,34 +432,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -461,11 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,78 +488,78 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -561,7 +568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -572,18 +579,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding ExcelReader utility methods
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marb6\git\repository\ExcelDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35BFDE7-9982-42DA-8F39-36B3F0A4293F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A642E69-9A62-4CC2-8E77-013C6F2C4DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -421,6 +421,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -465,135 +596,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added reportng and implementing custom listeners
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marb6\git\repository\ExcelDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A642E69-9A62-4CC2-8E77-013C6F2C4DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44CFBEB-B6D4-40CE-A562-BF1D2E257B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -44,9 +44,6 @@
     <t>alerttext</t>
   </si>
   <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
     <t>customer</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>runmode</t>
   </si>
   <si>
     <t>Dave</t>
@@ -422,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,76 +434,49 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -532,18 +496,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -555,42 +519,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>